<commit_message>
mark the 12V line
</commit_message>
<xml_diff>
--- a/Comparing Mosfets.xlsx
+++ b/Comparing Mosfets.xlsx
@@ -216,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -263,6 +263,18 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,10 +305,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -607,7 +619,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31:J32"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,123 +635,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="40">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="50">
         <v>1.3</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33" t="s">
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="46"/>
       <c r="G6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="37"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="28">
+      <c r="B7" s="38">
         <v>0.04</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="15">
         <v>1.05</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="39">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="F7" s="29"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="16">
         <v>0.45</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="40">
         <v>0.03</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="40"/>
       <c r="J7" s="17">
         <v>0.75</v>
       </c>
@@ -817,7 +829,7 @@
         <v>78.850499999999883</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>11</v>
       </c>
@@ -859,83 +871,83 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="A11" s="18">
         <v>12</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="19">
         <f t="shared" si="0"/>
         <v>8.9552238805970141</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="20">
         <f t="shared" si="1"/>
         <v>3.2078413900646114</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="21">
         <f t="shared" si="6"/>
         <v>41.034374999999883</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="22">
         <f t="shared" si="2"/>
         <v>9.2059838895281931</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="23">
         <f t="shared" si="3"/>
         <v>0.29662548780987841</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="24">
         <f t="shared" si="7"/>
         <v>454.66935267858042</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="25">
         <f t="shared" si="4"/>
         <v>9.022556390977444</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="26">
         <f t="shared" si="5"/>
         <v>2.4421957148510312</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="27">
         <f t="shared" si="8"/>
         <v>54.528125000000138</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="28">
         <v>13</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="29">
         <f t="shared" si="0"/>
         <v>9.7014925373134329</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="30">
         <f t="shared" si="1"/>
         <v>3.7647582980619272</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="31">
         <f t="shared" si="6"/>
         <v>34.808875739644989</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="32">
         <f t="shared" si="2"/>
         <v>9.9731492136555424</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="33">
         <f t="shared" si="3"/>
         <v>0.34812296833243117</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="34">
         <f t="shared" si="7"/>
         <v>387.34400464919969</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="35">
         <f t="shared" si="4"/>
         <v>9.7744360902255636</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="36">
         <f t="shared" si="5"/>
         <v>2.8661880264571171</v>
       </c>
-      <c r="J12" s="27">
+      <c r="J12" s="37">
         <f t="shared" si="8"/>
         <v>46.350887573964549</v>
       </c>
@@ -1638,123 +1650,123 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="61.5" x14ac:dyDescent="0.9">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="40">
-        <v>1</v>
-      </c>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="50">
+        <v>2.8</v>
+      </c>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
     </row>
     <row r="33" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="32" t="s">
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="33" t="s">
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="35"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="36" t="s">
+      <c r="E35" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="46"/>
       <c r="G35" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H35" s="37" t="s">
+      <c r="H35" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I35" s="37"/>
+      <c r="I35" s="47"/>
       <c r="J35" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="28">
+      <c r="B36" s="38">
         <v>0.04</v>
       </c>
-      <c r="C36" s="28"/>
+      <c r="C36" s="38"/>
       <c r="D36" s="15">
         <v>1.05</v>
       </c>
-      <c r="E36" s="29">
+      <c r="E36" s="39">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="F36" s="29"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <v>0.45</v>
       </c>
-      <c r="H36" s="30">
+      <c r="H36" s="40">
         <v>0.03</v>
       </c>
-      <c r="I36" s="30"/>
+      <c r="I36" s="40"/>
       <c r="J36" s="17">
         <v>0.75</v>
       </c>
@@ -1797,39 +1809,39 @@
       </c>
       <c r="B38" s="3">
         <f t="shared" ref="B38:B58" si="9">$A38/($F$31+B$7)</f>
-        <v>9.615384615384615</v>
+        <v>3.5211267605633805</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" ref="C38:C58" si="10">($A38-($F$31*B38))*B38</f>
-        <v>3.6982248520710095</v>
+        <v>0.49593334655822507</v>
       </c>
       <c r="D38" s="5">
         <f>((175-40)/C38)-$D$7</f>
-        <v>35.453999999999965</v>
+        <v>271.16399999999862</v>
       </c>
       <c r="E38" s="11">
         <f t="shared" ref="E38:E58" si="11">$A38/($F$31+E$7)</f>
-        <v>9.9651220727453911</v>
+        <v>3.5669698591046912</v>
       </c>
       <c r="F38" s="12">
         <f t="shared" ref="F38:F58" si="12">($A38-($F$31*E38))*E38</f>
-        <v>0.34756280273651141</v>
+        <v>4.4531458915160041E-2</v>
       </c>
       <c r="G38" s="13">
         <f>((175-40)/F38)-$G$7</f>
-        <v>387.96901071428516</v>
+        <v>3031.114725000316</v>
       </c>
       <c r="H38" s="7">
         <f t="shared" ref="H38:H58" si="13">$A38/($F$31+H$7)</f>
-        <v>9.7087378640776691</v>
+        <v>3.5335689045936403</v>
       </c>
       <c r="I38" s="8">
         <f t="shared" ref="I38:I58" si="14">($A38-($F$31*H38))*H38</f>
-        <v>2.8277877274012702</v>
+        <v>0.37458327610532927</v>
       </c>
       <c r="J38" s="9">
         <f>((175-40)/I38)-$J$7</f>
-        <v>46.990499999999884</v>
+        <v>359.65050000000343</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1838,39 +1850,39 @@
       </c>
       <c r="B39" s="3">
         <f t="shared" si="9"/>
-        <v>10.576923076923077</v>
+        <v>3.8732394366197185</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="10"/>
-        <v>4.4748520710059196</v>
+        <v>0.60007934933544682</v>
       </c>
       <c r="D39" s="5">
         <f t="shared" ref="D39:D58" si="15">((175-40)/C39)-$D$7</f>
-        <v>29.118595041322298</v>
+        <v>223.92024793388521</v>
       </c>
       <c r="E39" s="11">
         <f t="shared" si="11"/>
-        <v>10.961634280019929</v>
+        <v>3.9236668450151599</v>
       </c>
       <c r="F39" s="12">
         <f t="shared" si="12"/>
-        <v>0.42055099131119045</v>
+        <v>5.3883065287348521E-2</v>
       </c>
       <c r="G39" s="13">
         <f t="shared" ref="G39:G58" si="16">((175-40)/F39)-$G$7</f>
-        <v>320.55744687130118</v>
+        <v>2504.975392562018</v>
       </c>
       <c r="H39" s="7">
         <f t="shared" si="13"/>
-        <v>10.679611650485437</v>
+        <v>3.8869257950530041</v>
       </c>
       <c r="I39" s="8">
         <f t="shared" si="14"/>
-        <v>3.4216231501555221</v>
+        <v>0.4532457640874491</v>
       </c>
       <c r="J39" s="9">
         <f t="shared" ref="J39:J58" si="17">((175-40)/I39)-$J$7</f>
-        <v>38.704958677686022</v>
+        <v>297.10165289256435</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1879,39 +1891,39 @@
       </c>
       <c r="B40" s="19">
         <f t="shared" si="9"/>
-        <v>11.538461538461538</v>
+        <v>4.2253521126760569</v>
       </c>
       <c r="C40" s="20">
         <f t="shared" si="10"/>
-        <v>5.32544378698225</v>
+        <v>0.71414401904383962</v>
       </c>
       <c r="D40" s="21">
         <f t="shared" si="15"/>
-        <v>24.299999999999994</v>
+        <v>187.98750000000021</v>
       </c>
       <c r="E40" s="22">
         <f t="shared" si="11"/>
-        <v>11.958146487294469</v>
+        <v>4.2803638309256291</v>
       </c>
       <c r="F40" s="23">
         <f t="shared" si="12"/>
-        <v>0.50049043594058062</v>
+        <v>6.4125300837833493E-2</v>
       </c>
       <c r="G40" s="24">
         <f t="shared" si="16"/>
-        <v>269.28542410714022</v>
+        <v>2104.8032812501197</v>
       </c>
       <c r="H40" s="25">
         <f t="shared" si="13"/>
-        <v>11.650485436893204</v>
+        <v>4.2402826855123683</v>
       </c>
       <c r="I40" s="26">
         <f t="shared" si="14"/>
-        <v>4.0720143274578167</v>
+        <v>0.53939991759167571</v>
       </c>
       <c r="J40" s="27">
         <f t="shared" si="17"/>
-        <v>32.403125000000017</v>
+        <v>249.52812500000164</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1920,39 +1932,39 @@
       </c>
       <c r="B41" s="3">
         <f t="shared" si="9"/>
-        <v>12.5</v>
+        <v>4.5774647887323949</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="10"/>
-        <v>6.25</v>
+        <v>0.83812735568338903</v>
       </c>
       <c r="D41" s="5">
         <f t="shared" si="15"/>
-        <v>20.55</v>
+        <v>160.02337278106646</v>
       </c>
       <c r="E41" s="11">
         <f t="shared" si="11"/>
-        <v>12.954658694569007</v>
+        <v>4.6370608168360983</v>
       </c>
       <c r="F41" s="12">
         <f t="shared" si="12"/>
-        <v>0.58738113662472258</v>
+        <v>7.5258165566621293E-2</v>
       </c>
       <c r="G41" s="13">
         <f t="shared" si="16"/>
-        <v>229.38373415045743</v>
+        <v>1793.3752810652559</v>
       </c>
       <c r="H41" s="7">
         <f t="shared" si="13"/>
-        <v>12.621359223300971</v>
+        <v>4.5936395759717321</v>
       </c>
       <c r="I41" s="8">
         <f t="shared" si="14"/>
-        <v>4.7789612593081383</v>
+        <v>0.63304573661800889</v>
       </c>
       <c r="J41" s="9">
         <f t="shared" si="17"/>
-        <v>27.498816568047314</v>
+        <v>212.50473372781184</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1961,39 +1973,39 @@
       </c>
       <c r="B42" s="3">
         <f t="shared" si="9"/>
-        <v>13.461538461538462</v>
+        <v>4.9295774647887329</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="10"/>
-        <v>7.2485207100591698</v>
+        <v>0.97202935925411071</v>
       </c>
       <c r="D42" s="5">
         <f t="shared" si="15"/>
-        <v>17.574489795918371</v>
+        <v>137.83469387755179</v>
       </c>
       <c r="E42" s="11">
         <f t="shared" si="11"/>
-        <v>13.951170901843547</v>
+        <v>4.9937578027465674</v>
       </c>
       <c r="F42" s="12">
         <f t="shared" si="12"/>
-        <v>0.68122309336357223</v>
+        <v>8.7281659473720768E-2</v>
       </c>
       <c r="G42" s="13">
         <f t="shared" si="16"/>
-        <v>197.72296465014261</v>
+        <v>1546.2666964286068</v>
       </c>
       <c r="H42" s="7">
         <f t="shared" si="13"/>
-        <v>13.592233009708737</v>
+        <v>4.9469964664310959</v>
       </c>
       <c r="I42" s="8">
         <f t="shared" si="14"/>
-        <v>5.5424639457064853</v>
+        <v>0.73418322116644885</v>
       </c>
       <c r="J42" s="9">
         <f t="shared" si="17"/>
-        <v>23.607397959183633</v>
+        <v>183.12780612244984</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2002,39 +2014,39 @@
       </c>
       <c r="B43" s="3">
         <f t="shared" si="9"/>
-        <v>14.423076923076923</v>
+        <v>5.2816901408450709</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="10"/>
-        <v>8.3210059171597592</v>
+        <v>1.115850029755997</v>
       </c>
       <c r="D43" s="5">
         <f t="shared" si="15"/>
-        <v>15.174000000000007</v>
+        <v>119.93400000000041</v>
       </c>
       <c r="E43" s="11">
         <f t="shared" si="11"/>
-        <v>14.947683109118087</v>
+        <v>5.3504547886570366</v>
       </c>
       <c r="F43" s="12">
         <f t="shared" si="12"/>
-        <v>0.78201630615715068</v>
+        <v>0.10019578255911483</v>
       </c>
       <c r="G43" s="13">
         <f t="shared" si="16"/>
-        <v>172.18067142857117</v>
+        <v>1346.9121000000764</v>
       </c>
       <c r="H43" s="7">
         <f t="shared" si="13"/>
-        <v>14.563106796116504</v>
+        <v>5.3003533568904597</v>
       </c>
       <c r="I43" s="8">
         <f t="shared" si="14"/>
-        <v>6.3625223866528584</v>
+        <v>0.84281237123699548</v>
       </c>
       <c r="J43" s="9">
         <f t="shared" si="17"/>
-        <v>20.467999999999947</v>
+        <v>159.42800000000065</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2043,39 +2055,39 @@
       </c>
       <c r="B44" s="3">
         <f t="shared" si="9"/>
-        <v>15.384615384615383</v>
+        <v>5.6338028169014089</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="10"/>
-        <v>9.4674556213017951</v>
+        <v>1.2695893671890481</v>
       </c>
       <c r="D44" s="5">
         <f t="shared" si="15"/>
-        <v>13.209374999999969</v>
+        <v>105.28359375000014</v>
       </c>
       <c r="E44" s="11">
         <f t="shared" si="11"/>
-        <v>15.944195316392625</v>
+        <v>5.7071517745675058</v>
       </c>
       <c r="F44" s="12">
         <f t="shared" si="12"/>
-        <v>0.88976077500548612</v>
+        <v>0.11400053482281172</v>
       </c>
       <c r="G44" s="13">
         <f t="shared" si="16"/>
-        <v>151.27617606026476</v>
+        <v>1183.7549707032272</v>
       </c>
       <c r="H44" s="7">
         <f t="shared" si="13"/>
-        <v>15.533980582524272</v>
+        <v>5.6537102473498244</v>
       </c>
       <c r="I44" s="8">
         <f t="shared" si="14"/>
-        <v>7.2391365821472302</v>
+        <v>0.95893318682963891</v>
       </c>
       <c r="J44" s="9">
         <f t="shared" si="17"/>
-        <v>17.898632812500008</v>
+        <v>140.03144531250192</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2084,39 +2096,39 @@
       </c>
       <c r="B45" s="3">
         <f t="shared" si="9"/>
-        <v>16.346153846153847</v>
+        <v>5.9859154929577469</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="10"/>
-        <v>10.687869822485199</v>
+        <v>1.4332473715532534</v>
       </c>
       <c r="D45" s="5">
         <f t="shared" si="15"/>
-        <v>11.58114186851212</v>
+        <v>93.141695501730752</v>
       </c>
       <c r="E45" s="11">
         <f t="shared" si="11"/>
-        <v>16.940707523667164</v>
+        <v>6.0638487604779749</v>
       </c>
       <c r="F45" s="12">
         <f t="shared" si="12"/>
-        <v>1.0044564999085239</v>
+        <v>0.12869591626481144</v>
       </c>
       <c r="G45" s="13">
         <f t="shared" si="16"/>
-        <v>133.95104176964804</v>
+        <v>1048.5343339101526</v>
       </c>
       <c r="H45" s="7">
         <f t="shared" si="13"/>
-        <v>16.504854368932037</v>
+        <v>6.0070671378091882</v>
       </c>
       <c r="I45" s="8">
         <f t="shared" si="14"/>
-        <v>8.1723065321896815</v>
+        <v>1.0825456679443983</v>
       </c>
       <c r="J45" s="9">
         <f t="shared" si="17"/>
-        <v>15.76920415224907</v>
+        <v>123.95605536332336</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2125,39 +2137,39 @@
       </c>
       <c r="B46" s="3">
         <f t="shared" si="9"/>
-        <v>17.307692307692307</v>
+        <v>6.3380281690140849</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="10"/>
-        <v>11.982248520710078</v>
+        <v>1.6068240428486447</v>
       </c>
       <c r="D46" s="5">
         <f t="shared" si="15"/>
-        <v>10.216666666666649</v>
+        <v>82.966666666666484</v>
       </c>
       <c r="E46" s="11">
         <f t="shared" si="11"/>
-        <v>17.937219730941703</v>
+        <v>6.4205457463884441</v>
       </c>
       <c r="F46" s="12">
         <f t="shared" si="12"/>
-        <v>1.1261034808663224</v>
+        <v>0.14428192688512537</v>
       </c>
       <c r="G46" s="13">
         <f t="shared" si="16"/>
-        <v>119.43241071428282</v>
+        <v>935.21812500005308</v>
       </c>
       <c r="H46" s="7">
         <f t="shared" si="13"/>
-        <v>17.475728155339805</v>
+        <v>6.360424028268552</v>
       </c>
       <c r="I46" s="8">
         <f t="shared" si="14"/>
-        <v>9.162032236780103</v>
+        <v>1.2136498145812644</v>
       </c>
       <c r="J46" s="9">
         <f t="shared" si="17"/>
-        <v>13.984722222222205</v>
+        <v>110.4847222222235</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2166,39 +2178,39 @@
       </c>
       <c r="B47" s="3">
         <f t="shared" si="9"/>
-        <v>18.26923076923077</v>
+        <v>6.6901408450704229</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="10"/>
-        <v>13.350591715976316</v>
+        <v>1.7903193810751783</v>
       </c>
       <c r="D47" s="5">
         <f t="shared" si="15"/>
-        <v>9.0619113573407315</v>
+        <v>74.355540166205202</v>
       </c>
       <c r="E47" s="11">
         <f t="shared" si="11"/>
-        <v>18.933731938216241</v>
+        <v>6.7772427322989133</v>
       </c>
       <c r="F47" s="12">
         <f t="shared" si="12"/>
-        <v>1.2547017178788531</v>
+        <v>0.16075856668371932</v>
       </c>
       <c r="G47" s="13">
         <f t="shared" si="16"/>
-        <v>107.14529382666775</v>
+        <v>839.31862188378784</v>
       </c>
       <c r="H47" s="7">
         <f t="shared" si="13"/>
-        <v>18.446601941747574</v>
+        <v>6.7137809187279158</v>
       </c>
       <c r="I47" s="8">
         <f t="shared" si="14"/>
-        <v>10.208313695918548</v>
+        <v>1.3522456267402374</v>
       </c>
       <c r="J47" s="9">
         <f t="shared" si="17"/>
-        <v>12.474515235457078</v>
+        <v>99.083933518006575</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2207,39 +2219,39 @@
       </c>
       <c r="B48" s="3">
         <f t="shared" si="9"/>
-        <v>19.23076923076923</v>
+        <v>7.042253521126761</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="10"/>
-        <v>14.792899408284038</v>
+        <v>1.9837333862329003</v>
       </c>
       <c r="D48" s="5">
         <f t="shared" si="15"/>
-        <v>8.0759999999999899</v>
+        <v>67.003499999999661</v>
       </c>
       <c r="E48" s="11">
         <f t="shared" si="11"/>
-        <v>19.930244145490782</v>
+        <v>7.1339397182093824</v>
       </c>
       <c r="F48" s="12">
         <f t="shared" si="12"/>
-        <v>1.3902512109460456</v>
+        <v>0.17812583566064016</v>
       </c>
       <c r="G48" s="13">
         <f t="shared" si="16"/>
-        <v>96.654752678571285</v>
+        <v>757.4411812500789</v>
       </c>
       <c r="H48" s="7">
         <f t="shared" si="13"/>
-        <v>19.417475728155338</v>
+        <v>7.0671378091872805</v>
       </c>
       <c r="I48" s="8">
         <f t="shared" si="14"/>
-        <v>11.311150909605081</v>
+        <v>1.4983331044213171</v>
       </c>
       <c r="J48" s="9">
         <f t="shared" si="17"/>
-        <v>11.185124999999971</v>
+        <v>89.350125000000858</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2248,39 +2260,39 @@
       </c>
       <c r="B49" s="3">
         <f t="shared" si="9"/>
-        <v>20.19230769230769</v>
+        <v>7.394366197183099</v>
       </c>
       <c r="C49" s="4">
         <f t="shared" si="10"/>
-        <v>16.309171597633185</v>
+        <v>2.1870660583217618</v>
       </c>
       <c r="D49" s="5">
         <f t="shared" si="15"/>
-        <v>7.2275510204081383</v>
+        <v>60.676530612244896</v>
       </c>
       <c r="E49" s="11">
         <f t="shared" si="11"/>
-        <v>20.92675635276532</v>
+        <v>7.4906367041198507</v>
       </c>
       <c r="F49" s="12">
         <f t="shared" si="12"/>
-        <v>1.5327519600680375</v>
+        <v>0.19638373381586507</v>
       </c>
       <c r="G49" s="13">
         <f t="shared" si="16"/>
-        <v>87.626873177841162</v>
+        <v>686.97964285718183</v>
       </c>
       <c r="H49" s="7">
         <f t="shared" si="13"/>
-        <v>20.388349514563107</v>
+        <v>7.4204946996466443</v>
       </c>
       <c r="I49" s="8">
         <f t="shared" si="14"/>
-        <v>12.470543877839573</v>
+        <v>1.6519122476245034</v>
       </c>
       <c r="J49" s="9">
         <f t="shared" si="17"/>
-        <v>10.075510204081631</v>
+        <v>80.973469387755813</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2289,39 +2301,39 @@
       </c>
       <c r="B50" s="3">
         <f t="shared" si="9"/>
-        <v>21.153846153846153</v>
+        <v>7.746478873239437</v>
       </c>
       <c r="C50" s="4">
         <f t="shared" si="10"/>
-        <v>17.899408284023679</v>
+        <v>2.4003173973417873</v>
       </c>
       <c r="D50" s="5">
         <f t="shared" si="15"/>
-        <v>6.4921487603305748</v>
+        <v>55.192561983471307</v>
       </c>
       <c r="E50" s="11">
         <f t="shared" si="11"/>
-        <v>21.923268560039858</v>
+        <v>7.8473336900303199</v>
       </c>
       <c r="F50" s="12">
         <f t="shared" si="12"/>
-        <v>1.6822039652447618</v>
+        <v>0.21553226114939408</v>
       </c>
       <c r="G50" s="13">
         <f t="shared" si="16"/>
-        <v>79.80186171782529</v>
+        <v>625.90634814050441</v>
       </c>
       <c r="H50" s="7">
         <f t="shared" si="13"/>
-        <v>21.359223300970875</v>
+        <v>7.7738515901060081</v>
       </c>
       <c r="I50" s="8">
         <f t="shared" si="14"/>
-        <v>13.686492600622088</v>
+        <v>1.8129830563497964</v>
       </c>
       <c r="J50" s="9">
         <f t="shared" si="17"/>
-        <v>9.1137396694215056</v>
+        <v>73.712913223141086</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2330,39 +2342,39 @@
       </c>
       <c r="B51" s="3">
         <f t="shared" si="9"/>
-        <v>22.115384615384613</v>
+        <v>8.0985915492957758</v>
       </c>
       <c r="C51" s="4">
         <f t="shared" si="10"/>
-        <v>19.563609467455667</v>
+        <v>2.6234874032929762</v>
       </c>
       <c r="D51" s="5">
         <f t="shared" si="15"/>
-        <v>5.8505671077504564</v>
+        <v>50.40822306238227</v>
       </c>
       <c r="E51" s="11">
         <f t="shared" si="11"/>
-        <v>22.9197807673144</v>
+        <v>8.2040306759407891</v>
       </c>
       <c r="F51" s="12">
         <f t="shared" si="12"/>
-        <v>1.8386072264761373</v>
+        <v>0.23557141766122719</v>
       </c>
       <c r="G51" s="13">
         <f t="shared" si="16"/>
-        <v>72.975143802322648</v>
+        <v>572.62461720225372</v>
       </c>
       <c r="H51" s="7">
         <f t="shared" si="13"/>
-        <v>22.33009708737864</v>
+        <v>8.1272084805653719</v>
       </c>
       <c r="I51" s="8">
         <f t="shared" si="14"/>
-        <v>14.958997077952704</v>
+        <v>1.9815455305971961</v>
       </c>
       <c r="J51" s="9">
         <f t="shared" si="17"/>
-        <v>8.2746691871455447</v>
+        <v>67.378638941399359</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2371,39 +2383,39 @@
       </c>
       <c r="B52" s="19">
         <f t="shared" si="9"/>
-        <v>23.076923076923077</v>
+        <v>8.4507042253521139</v>
       </c>
       <c r="C52" s="20">
         <f t="shared" si="10"/>
-        <v>21.301775147929</v>
+        <v>2.8565760761753585</v>
       </c>
       <c r="D52" s="21">
         <f t="shared" si="15"/>
-        <v>5.2874999999999988</v>
+        <v>46.209375000000058</v>
       </c>
       <c r="E52" s="22">
         <f t="shared" si="11"/>
-        <v>23.916292974588938</v>
+        <v>8.5607276618512582</v>
       </c>
       <c r="F52" s="23">
         <f t="shared" si="12"/>
-        <v>2.0019617437623225</v>
+        <v>0.25650120335133397</v>
       </c>
       <c r="G52" s="24">
         <f t="shared" si="16"/>
-        <v>66.983856026785048</v>
+        <v>525.86332031252982</v>
       </c>
       <c r="H52" s="25">
         <f t="shared" si="13"/>
-        <v>23.300970873786408</v>
+        <v>8.4805653710247366</v>
       </c>
       <c r="I52" s="26">
         <f t="shared" si="14"/>
-        <v>16.288057309831267</v>
+        <v>2.1575996703667029</v>
       </c>
       <c r="J52" s="27">
         <f t="shared" si="17"/>
-        <v>7.5382812500000043</v>
+        <v>61.819531250000409</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -2412,39 +2424,39 @@
       </c>
       <c r="B53" s="3">
         <f t="shared" si="9"/>
-        <v>24.038461538461537</v>
+        <v>8.8028169014084519</v>
       </c>
       <c r="C53" s="4">
         <f t="shared" si="10"/>
-        <v>23.113905325443831</v>
+        <v>3.0995834159888758</v>
       </c>
       <c r="D53" s="5">
         <f t="shared" si="15"/>
-        <v>4.7906399999999891</v>
+        <v>42.504240000000216</v>
       </c>
       <c r="E53" s="11">
         <f t="shared" si="11"/>
-        <v>24.912805181863476</v>
+        <v>8.9174246477617274</v>
       </c>
       <c r="F53" s="12">
         <f t="shared" si="12"/>
-        <v>2.1722675171032404</v>
+        <v>0.27832161821977397</v>
       </c>
       <c r="G53" s="13">
         <f t="shared" si="16"/>
-        <v>61.69704171428436</v>
+        <v>484.60035600000919</v>
       </c>
       <c r="H53" s="7">
         <f t="shared" si="13"/>
-        <v>24.271844660194173</v>
+        <v>8.8339222614840995</v>
       </c>
       <c r="I53" s="8">
         <f t="shared" si="14"/>
-        <v>17.673673296257938</v>
+        <v>2.3411454756583154</v>
       </c>
       <c r="J53" s="9">
         <f t="shared" si="17"/>
-        <v>6.8884799999999808</v>
+        <v>56.914080000000361</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -2453,39 +2465,39 @@
       </c>
       <c r="B54" s="3">
         <f t="shared" si="9"/>
-        <v>25</v>
+        <v>9.1549295774647899</v>
       </c>
       <c r="C54" s="4">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>3.3525094227335561</v>
       </c>
       <c r="D54" s="5">
         <f t="shared" si="15"/>
-        <v>4.3500000000000005</v>
+        <v>39.21834319526662</v>
       </c>
       <c r="E54" s="11">
         <f t="shared" si="11"/>
-        <v>25.909317389138014</v>
+        <v>9.2741216336721966</v>
       </c>
       <c r="F54" s="12">
         <f t="shared" si="12"/>
-        <v>2.3495245464988903</v>
+        <v>0.30103266226648517</v>
       </c>
       <c r="G54" s="13">
         <f t="shared" si="16"/>
-        <v>57.008433537614351</v>
+        <v>448.00632026631399</v>
       </c>
       <c r="H54" s="7">
         <f t="shared" si="13"/>
-        <v>25.242718446601941</v>
+        <v>9.1872791519434642</v>
       </c>
       <c r="I54" s="8">
         <f t="shared" si="14"/>
-        <v>19.115845037232553</v>
+        <v>2.5321829464720356</v>
       </c>
       <c r="J54" s="9">
         <f t="shared" si="17"/>
-        <v>6.3122041420118284</v>
+        <v>52.56368343195296</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -2494,39 +2506,39 @@
       </c>
       <c r="B55" s="3">
         <f t="shared" si="9"/>
-        <v>25.96153846153846</v>
+        <v>9.5070422535211279</v>
       </c>
       <c r="C55" s="4">
         <f t="shared" si="10"/>
-        <v>26.960059171597674</v>
+        <v>3.6153540964094342</v>
       </c>
       <c r="D55" s="5">
         <f t="shared" si="15"/>
-        <v>3.9574074074074002</v>
+        <v>36.29074074074083</v>
       </c>
       <c r="E55" s="11">
         <f t="shared" si="11"/>
-        <v>26.905829596412556</v>
+        <v>9.6308186195826657</v>
       </c>
       <c r="F55" s="12">
         <f t="shared" si="12"/>
-        <v>2.5337328319491776</v>
+        <v>0.32463433549153209</v>
       </c>
       <c r="G55" s="13">
         <f t="shared" si="16"/>
-        <v>52.83107142857115</v>
+        <v>415.40250000002357</v>
       </c>
       <c r="H55" s="7">
         <f t="shared" si="13"/>
-        <v>26.21359223300971</v>
+        <v>9.5406360424028289</v>
       </c>
       <c r="I55" s="8">
         <f t="shared" si="14"/>
-        <v>20.614572532755187</v>
+        <v>2.7307120828078286</v>
       </c>
       <c r="J55" s="9">
         <f t="shared" si="17"/>
-        <v>5.7987654320987723</v>
+        <v>48.687654320988514</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -2535,39 +2547,39 @@
       </c>
       <c r="B56" s="3">
         <f t="shared" si="9"/>
-        <v>26.923076923076923</v>
+        <v>9.8591549295774659</v>
       </c>
       <c r="C56" s="4">
         <f t="shared" si="10"/>
-        <v>28.994082840236679</v>
+        <v>3.8881174370164429</v>
       </c>
       <c r="D56" s="5">
         <f t="shared" si="15"/>
-        <v>3.6061224489795931</v>
+        <v>33.671173469387952</v>
       </c>
       <c r="E56" s="11">
         <f t="shared" si="11"/>
-        <v>27.902341803687094</v>
+        <v>9.9875156054931349</v>
       </c>
       <c r="F56" s="12">
         <f t="shared" si="12"/>
-        <v>2.7248923734542889</v>
+        <v>0.34912663789488307</v>
       </c>
       <c r="G56" s="13">
         <f t="shared" si="16"/>
-        <v>49.093241162535648</v>
+        <v>386.22917410715172</v>
       </c>
       <c r="H56" s="7">
         <f t="shared" si="13"/>
-        <v>27.184466019417474</v>
+        <v>9.8939929328621918</v>
       </c>
       <c r="I56" s="8">
         <f t="shared" si="14"/>
-        <v>22.169855782825941</v>
+        <v>2.9367328846657954</v>
       </c>
       <c r="J56" s="9">
         <f t="shared" si="17"/>
-        <v>5.3393494897959082</v>
+        <v>45.21945153061246</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -2576,39 +2588,39 @@
       </c>
       <c r="B57" s="3">
         <f t="shared" si="9"/>
-        <v>27.884615384615383</v>
+        <v>10.211267605633804</v>
       </c>
       <c r="C57" s="4">
         <f t="shared" si="10"/>
-        <v>31.102071005917196</v>
+        <v>4.1707994445546515</v>
       </c>
       <c r="D57" s="5">
         <f t="shared" si="15"/>
-        <v>3.2905469678953576</v>
+        <v>31.317895362663496</v>
       </c>
       <c r="E57" s="11">
         <f t="shared" si="11"/>
-        <v>28.898854010961632</v>
+        <v>10.344212591403604</v>
       </c>
       <c r="F57" s="12">
         <f t="shared" si="12"/>
-        <v>2.9230031710141327</v>
+        <v>0.37450956947650144</v>
       </c>
       <c r="G57" s="13">
         <f t="shared" si="16"/>
-        <v>45.735375828094604</v>
+        <v>360.02142984545435</v>
       </c>
       <c r="H57" s="7">
         <f t="shared" si="13"/>
-        <v>28.155339805825243</v>
+        <v>10.247349823321557</v>
       </c>
       <c r="I57" s="8">
         <f t="shared" si="14"/>
-        <v>23.781694787444625</v>
+        <v>3.1502453520458356</v>
       </c>
       <c r="J57" s="9">
         <f t="shared" si="17"/>
-        <v>4.926634958382877</v>
+        <v>42.103804994054883</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -2617,39 +2629,39 @@
       </c>
       <c r="B58" s="3">
         <f t="shared" si="9"/>
-        <v>28.846153846153847</v>
+        <v>10.563380281690142</v>
       </c>
       <c r="C58" s="4">
         <f t="shared" si="10"/>
-        <v>33.284023668639037</v>
+        <v>4.463400119023988</v>
       </c>
       <c r="D58" s="5">
         <f t="shared" si="15"/>
-        <v>3.006000000000002</v>
+        <v>29.196000000000101</v>
       </c>
       <c r="E58" s="11">
         <f t="shared" si="11"/>
-        <v>29.895366218236173</v>
+        <v>10.700909577314073</v>
       </c>
       <c r="F58" s="12">
         <f t="shared" si="12"/>
-        <v>3.1280652246286027</v>
+        <v>0.40078313023645934</v>
       </c>
       <c r="G58" s="13">
         <f t="shared" si="16"/>
-        <v>42.707667857142788</v>
+        <v>336.39052500001912</v>
       </c>
       <c r="H58" s="7">
         <f t="shared" si="13"/>
-        <v>29.126213592233007</v>
+        <v>10.600706713780919</v>
       </c>
       <c r="I58" s="8">
         <f t="shared" si="14"/>
-        <v>25.450089546611434</v>
+        <v>3.3712494849479819</v>
       </c>
       <c r="J58" s="9">
         <f t="shared" si="17"/>
-        <v>4.5544999999999867</v>
+        <v>39.294500000000163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>